<commit_message>
refactor: update database schema for knowledge data to support pre-filtering
rebuild assets

rebuild knowledge
</commit_message>
<xml_diff>
--- a/knowledge/proprietary/test-excel-file.xlsx
+++ b/knowledge/proprietary/test-excel-file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charnould/GitHub/pierre/knowledge/proprietary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7C0CE4-AEC9-CE4D-98C6-1F96D1925F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA54885-8A9C-374D-8419-72BB5831167A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="1800" windowWidth="29040" windowHeight="15840" xr2:uid="{CBB88DEE-1036-475E-A925-BEA641FFA437}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="193">
   <si>
     <t>R+3</t>
   </si>
@@ -634,6 +634,15 @@
   </si>
   <si>
     <t>dmalfoy@pierre-habitat.fr</t>
+  </si>
+  <si>
+    <t>Poliglot</t>
+  </si>
+  <si>
+    <t>Plombier Fuitedo</t>
+  </si>
+  <si>
+    <t>Individuel</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1191,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1464,7 +1473,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>28</v>
+        <v>190</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>43</v>
@@ -1530,7 +1539,7 @@
         <v>43</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>38</v>
+        <v>192</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>186</v>
@@ -1587,7 +1596,7 @@
         <v>29</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>43</v>
+        <v>191</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>38</v>
@@ -5237,9 +5246,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5387,19 +5399,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEEDC912-A8BF-403A-A187-0254262D8DF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0CA54FD-799C-4637-92AD-9D4F60478507}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5423,9 +5431,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0CA54FD-799C-4637-92AD-9D4F60478507}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEEDC912-A8BF-403A-A187-0254262D8DF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>